<commit_message>
add gene annotations for another module
</commit_message>
<xml_diff>
--- a/docs/asset/1213_cd_ibd_Allergy_coloc_module_david_query.xlsx
+++ b/docs/asset/1213_cd_ibd_Allergy_coloc_module_david_query.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liliwang/Documents/R/GradLog/docs/asset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liliwang/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38B000B9-B7A9-6D40-A1EF-CEE55E2729C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2C3FC8-44C7-9345-AEB5-94EEAF12743A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="520" yWindow="1720" windowWidth="18420" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="module25" sheetId="1" r:id="rId1"/>
-    <sheet name="module153" sheetId="2" r:id="rId2"/>
-    <sheet name="module156" sheetId="3" r:id="rId3"/>
+    <sheet name="module51" sheetId="4" r:id="rId2"/>
+    <sheet name="module153" sheetId="2" r:id="rId3"/>
+    <sheet name="module156" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="619">
   <si>
     <t>ICMT</t>
   </si>
@@ -114,15 +115,9 @@
     <t>cytochrome b5 reductase like [Source:HGNC Symbol;Acc:HGNC:32220]</t>
   </si>
   <si>
-    <t>ENSG00000256407</t>
-  </si>
-  <si>
     <t>nan</t>
   </si>
   <si>
-    <t>novel transcript</t>
-  </si>
-  <si>
     <t>INADL</t>
   </si>
   <si>
@@ -156,12 +151,6 @@
     <t>GABPB2</t>
   </si>
   <si>
-    <t>ENSG00000104064</t>
-  </si>
-  <si>
-    <t>GA binding protein transcription factor subunit beta 1 [Source:HGNC Symbol;Acc:HGNC:4074]</t>
-  </si>
-  <si>
     <t>ENSG00000143458</t>
   </si>
   <si>
@@ -846,12 +835,6 @@
     <t>SLFN12L</t>
   </si>
   <si>
-    <t>ENSG00000205045</t>
-  </si>
-  <si>
-    <t>schlafen family member 12 like [Source:NCBI gene (formerly Entrezgene);Acc:100506736]</t>
-  </si>
-  <si>
     <t>ENSG00000286065</t>
   </si>
   <si>
@@ -1366,12 +1349,543 @@
   </si>
   <si>
     <t>zinc finger protein 43 [Source:HGNC Symbol;Acc:HGNC:13109]</t>
+  </si>
+  <si>
+    <t>ZNF595</t>
+  </si>
+  <si>
+    <t>ENSG00000272602</t>
+  </si>
+  <si>
+    <t>zinc finger protein 595 [Source:HGNC Symbol;Acc:HGNC:27196]</t>
+  </si>
+  <si>
+    <t>ZNF718</t>
+  </si>
+  <si>
+    <t>ENSG00000250312</t>
+  </si>
+  <si>
+    <t>zinc finger protein 718 [Source:HGNC Symbol;Acc:HGNC:26889]</t>
+  </si>
+  <si>
+    <t>ZNF107</t>
+  </si>
+  <si>
+    <t>ENSG00000196247</t>
+  </si>
+  <si>
+    <t>zinc finger protein 107 [Source:HGNC Symbol;Acc:HGNC:12887]</t>
+  </si>
+  <si>
+    <t>PHKB</t>
+  </si>
+  <si>
+    <t>ENSG00000102893</t>
+  </si>
+  <si>
+    <t>phosphorylase kinase regulatory subunit beta [Source:HGNC Symbol;Acc:HGNC:8927]</t>
+  </si>
+  <si>
+    <t>ZNF69</t>
+  </si>
+  <si>
+    <t>ENSG00000198429</t>
+  </si>
+  <si>
+    <t>zinc finger protein 69 [Source:HGNC Symbol;Acc:HGNC:13138]</t>
+  </si>
+  <si>
+    <t>ZNF763</t>
+  </si>
+  <si>
+    <t>ENSG00000197054</t>
+  </si>
+  <si>
+    <t>zinc finger protein 763 [Source:HGNC Symbol;Acc:HGNC:27614]</t>
+  </si>
+  <si>
+    <t>ZNF433</t>
+  </si>
+  <si>
+    <t>ENSG00000197647</t>
+  </si>
+  <si>
+    <t>zinc finger protein 433 [Source:HGNC Symbol;Acc:HGNC:20811]</t>
+  </si>
+  <si>
+    <t>ZNF44</t>
+  </si>
+  <si>
+    <t>ENSG00000197857</t>
+  </si>
+  <si>
+    <t>zinc finger protein 44 [Source:HGNC Symbol;Acc:HGNC:13110]</t>
+  </si>
+  <si>
+    <t>LINC00665</t>
+  </si>
+  <si>
+    <t>ENSG00000232677</t>
+  </si>
+  <si>
+    <t>long intergenic non-protein coding RNA 665 [Source:HGNC Symbol;Acc:HGNC:44323]</t>
+  </si>
+  <si>
+    <t>ZFP82</t>
+  </si>
+  <si>
+    <t>ENSG00000181007</t>
+  </si>
+  <si>
+    <t>ZFP82 zinc finger protein [Source:HGNC Symbol;Acc:HGNC:28682]</t>
+  </si>
+  <si>
+    <t>ZNF461</t>
+  </si>
+  <si>
+    <t>ENSG00000197808</t>
+  </si>
+  <si>
+    <t>zinc finger protein 461 [Source:HGNC Symbol;Acc:HGNC:21629]</t>
+  </si>
+  <si>
+    <t>ZNF585B</t>
+  </si>
+  <si>
+    <t>ENSG00000245680</t>
+  </si>
+  <si>
+    <t>zinc finger protein 585B [Source:HGNC Symbol;Acc:HGNC:30948]</t>
+  </si>
+  <si>
+    <t>HKR1</t>
+  </si>
+  <si>
+    <t>ZNF793</t>
+  </si>
+  <si>
+    <t>ENSG00000188227</t>
+  </si>
+  <si>
+    <t>zinc finger protein 793 [Source:HGNC Symbol;Acc:HGNC:33115]</t>
+  </si>
+  <si>
+    <t>ZNF404</t>
+  </si>
+  <si>
+    <t>ENSG00000176222</t>
+  </si>
+  <si>
+    <t>zinc finger protein 404 [Source:HGNC Symbol;Acc:HGNC:19417]</t>
+  </si>
+  <si>
+    <t>ZNF285</t>
+  </si>
+  <si>
+    <t>ENSG00000267508</t>
+  </si>
+  <si>
+    <t>zinc finger protein 285 [Source:HGNC Symbol;Acc:HGNC:13079]</t>
+  </si>
+  <si>
+    <t>ZNF577</t>
+  </si>
+  <si>
+    <t>ENSG00000161551</t>
+  </si>
+  <si>
+    <t>zinc finger protein 577 [Source:HGNC Symbol;Acc:HGNC:28673]</t>
+  </si>
+  <si>
+    <t>ZNF649</t>
+  </si>
+  <si>
+    <t>ENSG00000198093</t>
+  </si>
+  <si>
+    <t>zinc finger protein 649 [Source:HGNC Symbol;Acc:HGNC:25741]</t>
+  </si>
+  <si>
+    <t>ZNF880</t>
+  </si>
+  <si>
+    <t>ENSG00000221923</t>
+  </si>
+  <si>
+    <t>zinc finger protein 880 [Source:HGNC Symbol;Acc:HGNC:37249]</t>
+  </si>
+  <si>
+    <t>ZNF528</t>
+  </si>
+  <si>
+    <t>ENSG00000167555</t>
+  </si>
+  <si>
+    <t>zinc finger protein 528 [Source:HGNC Symbol;Acc:HGNC:29384]</t>
+  </si>
+  <si>
+    <t>ZNF578</t>
+  </si>
+  <si>
+    <t>ENSG00000258405</t>
+  </si>
+  <si>
+    <t>zinc finger protein 578 [Source:HGNC Symbol;Acc:HGNC:26449]</t>
+  </si>
+  <si>
+    <t>ZNF320</t>
+  </si>
+  <si>
+    <t>ENSG00000182986</t>
+  </si>
+  <si>
+    <t>zinc finger protein 320 [Source:HGNC Symbol;Acc:HGNC:13842]</t>
+  </si>
+  <si>
+    <t>ZNF160</t>
+  </si>
+  <si>
+    <t>ENSG00000170949</t>
+  </si>
+  <si>
+    <t>zinc finger protein 160 [Source:HGNC Symbol;Acc:HGNC:12948]</t>
+  </si>
+  <si>
+    <t>ZNF415</t>
+  </si>
+  <si>
+    <t>ENSG00000170954</t>
+  </si>
+  <si>
+    <t>zinc finger protein 415 [Source:HGNC Symbol;Acc:HGNC:20636]</t>
+  </si>
+  <si>
+    <t>ZNF347</t>
+  </si>
+  <si>
+    <t>ENSG00000197937</t>
+  </si>
+  <si>
+    <t>zinc finger protein 347 [Source:HGNC Symbol;Acc:HGNC:16447]</t>
+  </si>
+  <si>
+    <t>ZNF677</t>
+  </si>
+  <si>
+    <t>ENSG00000197928</t>
+  </si>
+  <si>
+    <t>zinc finger protein 677 [Source:HGNC Symbol;Acc:HGNC:28730]</t>
+  </si>
+  <si>
+    <t>ZNF525</t>
+  </si>
+  <si>
+    <t>ENSG00000203326</t>
+  </si>
+  <si>
+    <t>zinc finger protein 525 [Source:HGNC Symbol;Acc:HGNC:29423]</t>
+  </si>
+  <si>
+    <t>ZNF582-AS1</t>
+  </si>
+  <si>
+    <t>ZNF667</t>
+  </si>
+  <si>
+    <t>ENSG00000198046</t>
+  </si>
+  <si>
+    <t>zinc finger protein 667 [Source:HGNC Symbol;Acc:HGNC:28854]</t>
+  </si>
+  <si>
+    <t>ZNF667-AS1</t>
+  </si>
+  <si>
+    <t>ENSG00000166770</t>
+  </si>
+  <si>
+    <t>ZNF667 antisense RNA 1 (head to head) [Source:HGNC Symbol;Acc:HGNC:44321]</t>
+  </si>
+  <si>
+    <t>ZFP28</t>
+  </si>
+  <si>
+    <t>ENSG00000196867</t>
+  </si>
+  <si>
+    <t>ZFP28 zinc finger protein [Source:HGNC Symbol;Acc:HGNC:17801]</t>
+  </si>
+  <si>
+    <t>ZNF470</t>
+  </si>
+  <si>
+    <t>ENSG00000197016</t>
+  </si>
+  <si>
+    <t>zinc finger protein 470 [Source:HGNC Symbol;Acc:HGNC:22220]</t>
+  </si>
+  <si>
+    <t>ZNF835</t>
+  </si>
+  <si>
+    <t>ENSG00000127903</t>
+  </si>
+  <si>
+    <t>zinc finger protein 835 [Source:HGNC Symbol;Acc:HGNC:34332]</t>
+  </si>
+  <si>
+    <t>AURKC</t>
+  </si>
+  <si>
+    <t>ENSG00000105146</t>
+  </si>
+  <si>
+    <t>aurora kinase C [Source:HGNC Symbol;Acc:HGNC:11391]</t>
+  </si>
+  <si>
+    <t>ZNF304</t>
+  </si>
+  <si>
+    <t>ENSG00000131845</t>
+  </si>
+  <si>
+    <t>zinc finger protein 304 [Source:HGNC Symbol;Acc:HGNC:13505]</t>
+  </si>
+  <si>
+    <t>TRAPPC2P1</t>
+  </si>
+  <si>
+    <t>ZNF547</t>
+  </si>
+  <si>
+    <t>ENSG00000152433</t>
+  </si>
+  <si>
+    <t>zinc finger protein 547 [Source:HGNC Symbol;Acc:HGNC:26432]</t>
+  </si>
+  <si>
+    <t>ZNF548</t>
+  </si>
+  <si>
+    <t>ENSG00000188785</t>
+  </si>
+  <si>
+    <t>zinc finger protein 548 [Source:HGNC Symbol;Acc:HGNC:26561]</t>
+  </si>
+  <si>
+    <t>ZNF772</t>
+  </si>
+  <si>
+    <t>ENSG00000197128</t>
+  </si>
+  <si>
+    <t>zinc finger protein 772 [Source:HGNC Symbol;Acc:HGNC:33106]</t>
+  </si>
+  <si>
+    <t>ZNF419</t>
+  </si>
+  <si>
+    <t>ENSG00000105136</t>
+  </si>
+  <si>
+    <t>zinc finger protein 419 [Source:HGNC Symbol;Acc:HGNC:20648]</t>
+  </si>
+  <si>
+    <t>ZNF773</t>
+  </si>
+  <si>
+    <t>ENSG00000152439</t>
+  </si>
+  <si>
+    <t>zinc finger protein 773 [Source:HGNC Symbol;Acc:HGNC:30487]</t>
+  </si>
+  <si>
+    <t>ZNF549</t>
+  </si>
+  <si>
+    <t>ENSG00000121406</t>
+  </si>
+  <si>
+    <t>zinc finger protein 549 [Source:HGNC Symbol;Acc:HGNC:26632]</t>
+  </si>
+  <si>
+    <t>ZNF416</t>
+  </si>
+  <si>
+    <t>ENSG00000083817</t>
+  </si>
+  <si>
+    <t>zinc finger protein 416 [Source:HGNC Symbol;Acc:HGNC:20645]</t>
+  </si>
+  <si>
+    <t>ZIK1</t>
+  </si>
+  <si>
+    <t>ENSG00000171649</t>
+  </si>
+  <si>
+    <t>zinc finger protein interacting with K protein 1 [Source:HGNC Symbol;Acc:HGNC:33104]</t>
+  </si>
+  <si>
+    <t>ZNF530</t>
+  </si>
+  <si>
+    <t>ENSG00000183647</t>
+  </si>
+  <si>
+    <t>zinc finger protein 530 [Source:HGNC Symbol;Acc:HGNC:29297]</t>
+  </si>
+  <si>
+    <t>ZNF134</t>
+  </si>
+  <si>
+    <t>ENSG00000213762</t>
+  </si>
+  <si>
+    <t>zinc finger protein 134 [Source:HGNC Symbol;Acc:HGNC:12918]</t>
+  </si>
+  <si>
+    <t>ZNF211</t>
+  </si>
+  <si>
+    <t>ENSG00000121417</t>
+  </si>
+  <si>
+    <t>zinc finger protein 211 [Source:HGNC Symbol;Acc:HGNC:13003]</t>
+  </si>
+  <si>
+    <t>ZNF551</t>
+  </si>
+  <si>
+    <t>ENSG00000204519</t>
+  </si>
+  <si>
+    <t>zinc finger protein 551 [Source:HGNC Symbol;Acc:HGNC:25108]</t>
+  </si>
+  <si>
+    <t>ZNF776</t>
+  </si>
+  <si>
+    <t>ENSG00000152443</t>
+  </si>
+  <si>
+    <t>zinc finger protein 776 [Source:HGNC Symbol;Acc:HGNC:26765]</t>
+  </si>
+  <si>
+    <t>ZNF154</t>
+  </si>
+  <si>
+    <t>ENSG00000179909</t>
+  </si>
+  <si>
+    <t>zinc finger protein 154 [Source:HGNC Symbol;Acc:HGNC:12939]</t>
+  </si>
+  <si>
+    <t>ZNF671</t>
+  </si>
+  <si>
+    <t>ENSG00000083814</t>
+  </si>
+  <si>
+    <t>zinc finger protein 671 [Source:HGNC Symbol;Acc:HGNC:26279]</t>
+  </si>
+  <si>
+    <t>ZNF587B</t>
+  </si>
+  <si>
+    <t>ENSG00000269343</t>
+  </si>
+  <si>
+    <t>zinc finger protein 587B [Source:HGNC Symbol;Acc:HGNC:37142]</t>
+  </si>
+  <si>
+    <t>ZNF814</t>
+  </si>
+  <si>
+    <t>ENSG00000204514</t>
+  </si>
+  <si>
+    <t>zinc finger protein 814 [Source:HGNC Symbol;Acc:HGNC:33258]</t>
+  </si>
+  <si>
+    <t>ZNF418</t>
+  </si>
+  <si>
+    <t>ENSG00000196724</t>
+  </si>
+  <si>
+    <t>zinc finger protein 418 [Source:HGNC Symbol;Acc:HGNC:20647]</t>
+  </si>
+  <si>
+    <t>ZNF256</t>
+  </si>
+  <si>
+    <t>ENSG00000152454</t>
+  </si>
+  <si>
+    <t>zinc finger protein 256 [Source:HGNC Symbol;Acc:HGNC:13049]</t>
+  </si>
+  <si>
+    <t>ZNF606</t>
+  </si>
+  <si>
+    <t>ENSG00000166704</t>
+  </si>
+  <si>
+    <t>zinc finger protein 606 [Source:HGNC Symbol;Acc:HGNC:25879]</t>
+  </si>
+  <si>
+    <t>ZNF135</t>
+  </si>
+  <si>
+    <t>ENSG00000176293</t>
+  </si>
+  <si>
+    <t>zinc finger protein 135 [Source:HGNC Symbol;Acc:HGNC:12919]</t>
+  </si>
+  <si>
+    <t>ZSCAN18</t>
+  </si>
+  <si>
+    <t>ENSG00000121413</t>
+  </si>
+  <si>
+    <t>zinc finger and SCAN domain containing 18 [Source:HGNC Symbol;Acc:HGNC:21037]</t>
+  </si>
+  <si>
+    <t>ZNF329</t>
+  </si>
+  <si>
+    <t>ENSG00000181894</t>
+  </si>
+  <si>
+    <t>zinc finger protein 329 [Source:HGNC Symbol;Acc:HGNC:14209]</t>
+  </si>
+  <si>
+    <t>ZNF274</t>
+  </si>
+  <si>
+    <t>ENSG00000171606</t>
+  </si>
+  <si>
+    <t>zinc finger protein 274 [Source:HGNC Symbol;Acc:HGNC:13068]</t>
+  </si>
+  <si>
+    <t>ZNF544</t>
+  </si>
+  <si>
+    <t>ENSG00000198131</t>
+  </si>
+  <si>
+    <t>zinc finger protein 544 [Source:HGNC Symbol;Acc:HGNC:16759]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2205,15 +2719,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C126"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2329,266 +2844,266 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2607,32 +3122,32 @@
         <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2651,186 +3166,186 @@
         <v>112</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C44" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C49" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C53" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B54" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>159</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2849,758 +3364,725 @@
         <v>164</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="C58" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C59" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B60" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C60" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B61" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B62" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C62" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B63" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B65" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C65" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B66" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B67" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C67" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B68" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C68" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B69" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C69" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B70" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C70" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B71" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C71" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B72" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C72" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B73" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C73" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C74" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B75" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C75" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B76" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C76" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B77" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C77" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B78" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C78" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B79" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C79" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B80" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C80" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B81" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C81" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B82" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C82" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B83" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C83" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B84" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C84" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B85" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C85" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B86" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C86" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B87" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C87" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B89" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C89" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B90" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C90" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B91" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C91" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B92" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C92" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B93" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C93" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B94" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C94" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B95" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C95" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="B96" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C96" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B97" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C97" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B98" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C98" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B99" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C99" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B100" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C100" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B101" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C101" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B102" t="s">
-        <v>294</v>
+        <v>30</v>
       </c>
       <c r="C102" t="s">
-        <v>295</v>
+        <v>30</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B103" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C103" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B104" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C104" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B105" t="s">
-        <v>31</v>
+        <v>304</v>
       </c>
       <c r="C105" t="s">
-        <v>31</v>
+        <v>305</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B106" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C106" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B107" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C107" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B108" t="s">
-        <v>310</v>
+        <v>30</v>
       </c>
       <c r="C108" t="s">
-        <v>311</v>
+        <v>30</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B109" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C109" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B110" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C110" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B111" t="s">
-        <v>31</v>
+        <v>320</v>
       </c>
       <c r="C111" t="s">
-        <v>31</v>
+        <v>321</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B112" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C112" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B113" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C113" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B114" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C114" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B115" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C115" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B116" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C116" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B117" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C117" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B118" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C118" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B119" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C119" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B120" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C120" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B121" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C121" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B122" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="C122" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B123" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C123" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>355</v>
-      </c>
-      <c r="B124" t="s">
-        <v>356</v>
-      </c>
-      <c r="C124" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>358</v>
-      </c>
-      <c r="B125" t="s">
-        <v>359</v>
-      </c>
-      <c r="C125" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>361</v>
-      </c>
-      <c r="B126" t="s">
-        <v>362</v>
-      </c>
-      <c r="C126" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3609,178 +4091,1052 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43108585-5A94-9246-8368-25D292E3DDAF}">
+  <dimension ref="A1:D61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>445</v>
+      </c>
+      <c r="B2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" t="s">
+        <v>452</v>
+      </c>
+      <c r="C4" t="s">
+        <v>451</v>
+      </c>
+      <c r="D4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>454</v>
+      </c>
+      <c r="B5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C5" t="s">
+        <v>454</v>
+      </c>
+      <c r="D5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>457</v>
+      </c>
+      <c r="B6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C6" t="s">
+        <v>457</v>
+      </c>
+      <c r="D6" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>460</v>
+      </c>
+      <c r="B7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C7" t="s">
+        <v>460</v>
+      </c>
+      <c r="D7" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C8" t="s">
+        <v>463</v>
+      </c>
+      <c r="D8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>466</v>
+      </c>
+      <c r="B9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C9" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" t="s">
+        <v>470</v>
+      </c>
+      <c r="C10" t="s">
+        <v>469</v>
+      </c>
+      <c r="D10" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>472</v>
+      </c>
+      <c r="B11" t="s">
+        <v>473</v>
+      </c>
+      <c r="C11" t="s">
+        <v>472</v>
+      </c>
+      <c r="D11" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>475</v>
+      </c>
+      <c r="B12" t="s">
+        <v>476</v>
+      </c>
+      <c r="C12" t="s">
+        <v>475</v>
+      </c>
+      <c r="D12" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>478</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>479</v>
+      </c>
+      <c r="B14" t="s">
+        <v>480</v>
+      </c>
+      <c r="C14" t="s">
+        <v>479</v>
+      </c>
+      <c r="D14" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>482</v>
+      </c>
+      <c r="B15" t="s">
+        <v>483</v>
+      </c>
+      <c r="C15" t="s">
+        <v>482</v>
+      </c>
+      <c r="D15" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>485</v>
+      </c>
+      <c r="B16" t="s">
+        <v>486</v>
+      </c>
+      <c r="C16" t="s">
+        <v>485</v>
+      </c>
+      <c r="D16" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B17" t="s">
+        <v>489</v>
+      </c>
+      <c r="C17" t="s">
+        <v>488</v>
+      </c>
+      <c r="D17" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>491</v>
+      </c>
+      <c r="B18" t="s">
+        <v>492</v>
+      </c>
+      <c r="C18" t="s">
+        <v>491</v>
+      </c>
+      <c r="D18" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>494</v>
+      </c>
+      <c r="B19" t="s">
+        <v>495</v>
+      </c>
+      <c r="C19" t="s">
+        <v>494</v>
+      </c>
+      <c r="D19" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>497</v>
+      </c>
+      <c r="B20" t="s">
+        <v>498</v>
+      </c>
+      <c r="C20" t="s">
+        <v>497</v>
+      </c>
+      <c r="D20" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>500</v>
+      </c>
+      <c r="B21" t="s">
+        <v>501</v>
+      </c>
+      <c r="C21" t="s">
+        <v>500</v>
+      </c>
+      <c r="D21" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>503</v>
+      </c>
+      <c r="B22" t="s">
+        <v>504</v>
+      </c>
+      <c r="C22" t="s">
+        <v>503</v>
+      </c>
+      <c r="D22" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>506</v>
+      </c>
+      <c r="B23" t="s">
+        <v>507</v>
+      </c>
+      <c r="C23" t="s">
+        <v>506</v>
+      </c>
+      <c r="D23" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>509</v>
+      </c>
+      <c r="B24" t="s">
+        <v>510</v>
+      </c>
+      <c r="C24" t="s">
+        <v>509</v>
+      </c>
+      <c r="D24" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>512</v>
+      </c>
+      <c r="B25" t="s">
+        <v>513</v>
+      </c>
+      <c r="C25" t="s">
+        <v>512</v>
+      </c>
+      <c r="D25" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>515</v>
+      </c>
+      <c r="B26" t="s">
+        <v>516</v>
+      </c>
+      <c r="C26" t="s">
+        <v>515</v>
+      </c>
+      <c r="D26" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>518</v>
+      </c>
+      <c r="B27" t="s">
+        <v>519</v>
+      </c>
+      <c r="C27" t="s">
+        <v>518</v>
+      </c>
+      <c r="D27" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>521</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>522</v>
+      </c>
+      <c r="B29" t="s">
+        <v>523</v>
+      </c>
+      <c r="C29" t="s">
+        <v>522</v>
+      </c>
+      <c r="D29" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>525</v>
+      </c>
+      <c r="B30" t="s">
+        <v>526</v>
+      </c>
+      <c r="C30" t="s">
+        <v>525</v>
+      </c>
+      <c r="D30" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>528</v>
+      </c>
+      <c r="B31" t="s">
+        <v>529</v>
+      </c>
+      <c r="C31" t="s">
+        <v>528</v>
+      </c>
+      <c r="D31" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>531</v>
+      </c>
+      <c r="B32" t="s">
+        <v>532</v>
+      </c>
+      <c r="C32" t="s">
+        <v>531</v>
+      </c>
+      <c r="D32" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>534</v>
+      </c>
+      <c r="B33" t="s">
+        <v>535</v>
+      </c>
+      <c r="C33" t="s">
+        <v>534</v>
+      </c>
+      <c r="D33" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>537</v>
+      </c>
+      <c r="B34" t="s">
+        <v>538</v>
+      </c>
+      <c r="C34" t="s">
+        <v>537</v>
+      </c>
+      <c r="D34" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>540</v>
+      </c>
+      <c r="B35" t="s">
+        <v>541</v>
+      </c>
+      <c r="C35" t="s">
+        <v>540</v>
+      </c>
+      <c r="D35" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>543</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>544</v>
+      </c>
+      <c r="B37" t="s">
+        <v>545</v>
+      </c>
+      <c r="C37" t="s">
+        <v>544</v>
+      </c>
+      <c r="D37" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>547</v>
+      </c>
+      <c r="B38" t="s">
+        <v>548</v>
+      </c>
+      <c r="C38" t="s">
+        <v>547</v>
+      </c>
+      <c r="D38" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>550</v>
+      </c>
+      <c r="B39" t="s">
+        <v>551</v>
+      </c>
+      <c r="C39" t="s">
+        <v>550</v>
+      </c>
+      <c r="D39" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>553</v>
+      </c>
+      <c r="B40" t="s">
+        <v>554</v>
+      </c>
+      <c r="C40" t="s">
+        <v>553</v>
+      </c>
+      <c r="D40" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>556</v>
+      </c>
+      <c r="B41" t="s">
+        <v>557</v>
+      </c>
+      <c r="C41" t="s">
+        <v>556</v>
+      </c>
+      <c r="D41" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>559</v>
+      </c>
+      <c r="B42" t="s">
+        <v>560</v>
+      </c>
+      <c r="C42" t="s">
+        <v>559</v>
+      </c>
+      <c r="D42" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>562</v>
+      </c>
+      <c r="B43" t="s">
+        <v>563</v>
+      </c>
+      <c r="C43" t="s">
+        <v>562</v>
+      </c>
+      <c r="D43" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>565</v>
+      </c>
+      <c r="B44" t="s">
+        <v>566</v>
+      </c>
+      <c r="C44" t="s">
+        <v>565</v>
+      </c>
+      <c r="D44" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>568</v>
+      </c>
+      <c r="B45" t="s">
+        <v>569</v>
+      </c>
+      <c r="C45" t="s">
+        <v>568</v>
+      </c>
+      <c r="D45" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>571</v>
+      </c>
+      <c r="B46" t="s">
+        <v>572</v>
+      </c>
+      <c r="C46" t="s">
+        <v>571</v>
+      </c>
+      <c r="D46" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>574</v>
+      </c>
+      <c r="B47" t="s">
+        <v>575</v>
+      </c>
+      <c r="C47" t="s">
+        <v>574</v>
+      </c>
+      <c r="D47" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>577</v>
+      </c>
+      <c r="B48" t="s">
+        <v>578</v>
+      </c>
+      <c r="C48" t="s">
+        <v>577</v>
+      </c>
+      <c r="D48" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>580</v>
+      </c>
+      <c r="B49" t="s">
+        <v>581</v>
+      </c>
+      <c r="C49" t="s">
+        <v>580</v>
+      </c>
+      <c r="D49" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>583</v>
+      </c>
+      <c r="B50" t="s">
+        <v>584</v>
+      </c>
+      <c r="C50" t="s">
+        <v>583</v>
+      </c>
+      <c r="D50" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>586</v>
+      </c>
+      <c r="B51" t="s">
+        <v>587</v>
+      </c>
+      <c r="C51" t="s">
+        <v>586</v>
+      </c>
+      <c r="D51" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>589</v>
+      </c>
+      <c r="B52" t="s">
+        <v>590</v>
+      </c>
+      <c r="C52" t="s">
+        <v>589</v>
+      </c>
+      <c r="D52" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>592</v>
+      </c>
+      <c r="B53" t="s">
+        <v>593</v>
+      </c>
+      <c r="C53" t="s">
+        <v>592</v>
+      </c>
+      <c r="D53" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>595</v>
+      </c>
+      <c r="B54" t="s">
+        <v>596</v>
+      </c>
+      <c r="C54" t="s">
+        <v>595</v>
+      </c>
+      <c r="D54" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>598</v>
+      </c>
+      <c r="B55" t="s">
+        <v>599</v>
+      </c>
+      <c r="C55" t="s">
+        <v>598</v>
+      </c>
+      <c r="D55" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>601</v>
+      </c>
+      <c r="B56" t="s">
+        <v>602</v>
+      </c>
+      <c r="C56" t="s">
+        <v>601</v>
+      </c>
+      <c r="D56" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>604</v>
+      </c>
+      <c r="B57" t="s">
+        <v>605</v>
+      </c>
+      <c r="C57" t="s">
+        <v>604</v>
+      </c>
+      <c r="D57" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>607</v>
+      </c>
+      <c r="B58" t="s">
+        <v>608</v>
+      </c>
+      <c r="C58" t="s">
+        <v>607</v>
+      </c>
+      <c r="D58" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>610</v>
+      </c>
+      <c r="B59" t="s">
+        <v>611</v>
+      </c>
+      <c r="C59" t="s">
+        <v>610</v>
+      </c>
+      <c r="D59" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>613</v>
+      </c>
+      <c r="B60" t="s">
+        <v>614</v>
+      </c>
+      <c r="C60" t="s">
+        <v>613</v>
+      </c>
+      <c r="D60" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>616</v>
+      </c>
+      <c r="B61" t="s">
+        <v>617</v>
+      </c>
+      <c r="C61" t="s">
+        <v>616</v>
+      </c>
+      <c r="D61" t="s">
+        <v>618</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D1" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="D2" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="B3" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D3" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B4" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D4" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B5" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="D5" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="B6" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D6" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B7" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D7" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="B8" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D8" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B9" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D9" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B10" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D10" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B11" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="D11" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B12" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D12" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="B13" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D13" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B14" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="D14" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B15" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D15" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -3788,157 +5144,155 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D1" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D2" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="B3" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D3" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D4" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B5" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="B6" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D6" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="B7" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D7" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B8" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D8" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B9" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D9" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B10" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D10" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="B11" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="D11" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="B12" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D12" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B13" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D13" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>